<commit_message>
[jini] excel data edit in DB
엑셀 값이 변경되면 DB에도 반영이 된다.
</commit_message>
<xml_diff>
--- a/player_list.xlsx
+++ b/player_list.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>id</t>
   </si>
@@ -47,6 +47,9 @@
   </si>
   <si>
     <t>손흥민</t>
+  </si>
+  <si>
+    <t>박지성</t>
   </si>
 </sst>
 </file>
@@ -412,10 +415,10 @@
         <v>80.0</v>
       </c>
       <c r="F5" s="1">
-        <v>80.0</v>
+        <v>50.0</v>
       </c>
       <c r="G5" s="1">
-        <v>80.0</v>
+        <v>50.0</v>
       </c>
     </row>
     <row r="6">
@@ -439,6 +442,29 @@
       </c>
       <c r="G6" s="1">
         <v>99.0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1">
+        <v>7.0</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="1">
+        <v>80.0</v>
+      </c>
+      <c r="D7" s="1">
+        <v>80.0</v>
+      </c>
+      <c r="E7" s="1">
+        <v>80.0</v>
+      </c>
+      <c r="F7" s="1">
+        <v>80.0</v>
+      </c>
+      <c r="G7" s="1">
+        <v>80.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[jini] 데이터 삽입/변경 방법 수정 & Promise.allSettled() 사용
인덱스를 기준으로 엑셀과 DB에 삽입된 데이터를 비교하는 대신, ID를 기준으로 데이터를 비교.
또한 비동기 처리를 병렬로 실행하기 위해 Promise.allSettled()를 사용.
</commit_message>
<xml_diff>
--- a/player_list.xlsx
+++ b/player_list.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>id</t>
   </si>
@@ -40,6 +40,9 @@
     <t>해리 케인</t>
   </si>
   <si>
+    <t>테스트</t>
+  </si>
+  <si>
     <t>페이커</t>
   </si>
   <si>
@@ -50,6 +53,9 @@
   </si>
   <si>
     <t>박지성</t>
+  </si>
+  <si>
+    <t>테스트2</t>
   </si>
 </sst>
 </file>
@@ -377,94 +383,140 @@
     </row>
     <row r="4">
       <c r="A4" s="1">
-        <v>4.0</v>
+        <v>3.0</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C4" s="1">
-        <v>99.0</v>
+        <v>0.0</v>
       </c>
       <c r="D4" s="1">
-        <v>99.0</v>
+        <v>0.0</v>
       </c>
       <c r="E4" s="1">
-        <v>99.0</v>
+        <v>0.0</v>
       </c>
       <c r="F4" s="1">
-        <v>99.0</v>
+        <v>0.0</v>
       </c>
       <c r="G4" s="1">
-        <v>99.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1">
-        <v>5.0</v>
+        <v>4.0</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C5" s="1">
-        <v>80.0</v>
+        <v>99.0</v>
       </c>
       <c r="D5" s="1">
-        <v>80.0</v>
+        <v>99.0</v>
       </c>
       <c r="E5" s="1">
-        <v>80.0</v>
+        <v>99.0</v>
       </c>
       <c r="F5" s="1">
-        <v>50.0</v>
+        <v>99.0</v>
       </c>
       <c r="G5" s="1">
-        <v>50.0</v>
+        <v>99.0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1">
-        <v>6.0</v>
+        <v>5.0</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C6" s="1">
-        <v>99.0</v>
+        <v>50.0</v>
       </c>
       <c r="D6" s="1">
-        <v>99.0</v>
+        <v>50.0</v>
       </c>
       <c r="E6" s="1">
-        <v>99.0</v>
+        <v>50.0</v>
       </c>
       <c r="F6" s="1">
-        <v>99.0</v>
+        <v>50.0</v>
       </c>
       <c r="G6" s="1">
-        <v>99.0</v>
+        <v>50.0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1">
-        <v>7.0</v>
+        <v>6.0</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C7" s="1">
+        <v>99.0</v>
+      </c>
+      <c r="D7" s="1">
+        <v>99.0</v>
+      </c>
+      <c r="E7" s="1">
+        <v>99.0</v>
+      </c>
+      <c r="F7" s="1">
+        <v>99.0</v>
+      </c>
+      <c r="G7" s="1">
+        <v>99.0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1">
+        <v>7.0</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="1">
         <v>80.0</v>
       </c>
-      <c r="D7" s="1">
+      <c r="D8" s="1">
         <v>80.0</v>
       </c>
-      <c r="E7" s="1">
+      <c r="E8" s="1">
         <v>80.0</v>
       </c>
-      <c r="F7" s="1">
+      <c r="F8" s="1">
         <v>80.0</v>
       </c>
-      <c r="G7" s="1">
+      <c r="G8" s="1">
         <v>80.0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1">
+        <v>8.0</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="1">
+        <v>50.0</v>
+      </c>
+      <c r="D9" s="1">
+        <v>50.0</v>
+      </c>
+      <c r="E9" s="1">
+        <v>50.0</v>
+      </c>
+      <c r="F9" s="1">
+        <v>50.0</v>
+      </c>
+      <c r="G9" s="1">
+        <v>50.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>